<commit_message>
Estructura y acceso a la base
</commit_message>
<xml_diff>
--- a/VotingSystem_3b/src/test/resources/votacionesFisicas.xlsx
+++ b/VotingSystem_3b/src/test/resources/votacionesFisicas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11550" windowHeight="3690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>tipo voto</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Virtual</t>
+  </si>
+  <si>
+    <t>AST001</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,8 +399,8 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>12</v>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -413,8 +416,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>12</v>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>